<commit_message>
test: [PROD-12573] update empty fields cypress tests with multi spaces field
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers_empty_unauthorized_fields.xlsx
+++ b/cypress/fixtures/customers_empty_unauthorized_fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -104,15 +104,19 @@
   </si>
   <si>
     <t xml:space="preserve">13/04/2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -187,7 +191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +209,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,13 +233,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.76"/>
   </cols>
@@ -399,6 +407,26 @@
         <v>27</v>
       </c>
       <c r="F9" s="0" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>1.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test: adapt cypress stubbing to new runner endpoints
Co-authored-by: Tristan Huet <tristan.huet@cosmotech.com>
</commit_message>
<xml_diff>
--- a/cypress/fixtures/customers_empty_unauthorized_fields.xlsx
+++ b/cypress/fixtures/customers_empty_unauthorized_fields.xlsx
@@ -236,10 +236,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.76"/>
   </cols>
@@ -417,7 +417,8 @@
       <c r="B10" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="C10" s="5" t="b">
+      <c r="C10" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">

</xml_diff>